<commit_message>
Ano e mes de scrap dos dados pelo CVM -> automaticos
</commit_message>
<xml_diff>
--- a/tabela_rentabilidades.xlsx
+++ b/tabela_rentabilidades.xlsx
@@ -466,8 +466,10 @@
           <t>Constellation Ações FIC FIA</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>1.96</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1.96</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr"/>
     </row>
@@ -482,15 +484,11 @@
           <t>Núcleo Ações FIC FIA</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3.26</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>-13.66</t>
-        </is>
+      <c r="C3" t="n">
+        <v>3.26</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-13.66</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Arrumado constellation web scrap
</commit_message>
<xml_diff>
--- a/tabela_rentabilidades.xlsx
+++ b/tabela_rentabilidades.xlsx
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1.96</t>
+          <t>0,68</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -484,11 +484,15 @@
           <t>Núcleo Ações FIC FIA</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>3.26</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-13.66</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-12,02</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -502,11 +506,15 @@
           <t>Dynamo Cougar</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>2.83</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-18.43</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-0,01</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>-17,71</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>